<commit_message>
Commit atrasado de 30/08
</commit_message>
<xml_diff>
--- a/.Documentos/Estudos.xlsx
+++ b/.Documentos/Estudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Área de Trabalho\ESTUDOS\.Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43445852-DFE3-4FC6-B432-6DBC58BD32CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9479E6BD-FD02-4DB5-8274-ED32AE278AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="323">
   <si>
     <t>1. MICROECONOMIA</t>
   </si>
@@ -1094,7 +1094,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1372,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B313"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" zoomScale="95" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="95" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,36 +1883,57 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B101" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B102" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B103" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B104" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B105" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B106" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="B107" t="s">
         <v>196</v>
       </c>
@@ -2900,6 +2932,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A313">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit de 04/09 atrasado, fechei a materia de micro classica
</commit_message>
<xml_diff>
--- a/.Documentos/Estudos.xlsx
+++ b/.Documentos/Estudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Área de Trabalho\ESTUDOS\.Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9479E6BD-FD02-4DB5-8274-ED32AE278AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D209F6D6-5A99-4094-A7FB-6108B5C14F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conteúdo" sheetId="1" r:id="rId1"/>
@@ -1383,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B313"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="95" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView showGridLines="0" topLeftCell="A79" zoomScale="95" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83852407-83CC-4798-B7A5-2EEB7E8F38C0}">
   <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>